<commit_message>
UPDATE DASH BOARD CHANGES
</commit_message>
<xml_diff>
--- a/data/source1_camas/input/disponibilidad_camas_hospitalarias.xlsx
+++ b/data/source1_camas/input/disponibilidad_camas_hospitalarias.xlsx
@@ -407,11 +407,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E747"/>
+  <dimension ref="A1:E749"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A724" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I738" sqref="I738"/>
+      <selection pane="bottomLeft" activeCell="L739" sqref="L739"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12026,6 +12026,40 @@
         <v>0.76923076923076927</v>
       </c>
     </row>
+    <row r="748" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A748" s="20">
+        <v>44759</v>
+      </c>
+      <c r="B748">
+        <v>0.36842105263157893</v>
+      </c>
+      <c r="C748">
+        <v>0.25555555555555554</v>
+      </c>
+      <c r="D748">
+        <v>0.1164021164021164</v>
+      </c>
+      <c r="E748">
+        <v>0.61538461538461542</v>
+      </c>
+    </row>
+    <row r="749" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A749" s="20">
+        <v>44760</v>
+      </c>
+      <c r="B749">
+        <v>0.36842105263157893</v>
+      </c>
+      <c r="C749">
+        <v>0.25555555555555554</v>
+      </c>
+      <c r="D749">
+        <v>0.1164021164021164</v>
+      </c>
+      <c r="E749">
+        <v>0.61538461538461542</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>